<commit_message>
modificacion en  archivo APPMO-SP_ARP_v1.1.xlsx
</commit_message>
<xml_diff>
--- a/9°A/Administración de proyectos/RA_GestionRiegos_SM-ROOT/APPMO-SP_ARP_v1.1.xlsx
+++ b/9°A/Administración de proyectos/RA_GestionRiegos_SM-ROOT/APPMO-SP_ARP_v1.1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RA_GestionRiegos_SM-ROOT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cecy Tapia\Desktop\SM-ROOT\9°A\Administración de proyectos\RA_GestionRiegos_SM-ROOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="1" r:id="rId1"/>
@@ -414,9 +414,6 @@
     <t>Diseño de interfaces equivocadas o mal diseñadas</t>
   </si>
   <si>
-    <t>Rediseñar las interfaces con base  a los requerimientos de software</t>
-  </si>
-  <si>
     <t>Mal analisís de la base de datos del producto</t>
   </si>
   <si>
@@ -430,44 +427,47 @@
   </si>
   <si>
     <t>Redefinir la arquitectura lógica llevando a cabo un analisis produndo para lograr  relaciones de tablas correctas con base a los procesos de la empresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acoplar los requerimientos nuevos o cambios  existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </t>
+  </si>
+  <si>
+    <t>Comunicación</t>
+  </si>
+  <si>
+    <t>todos los entregables del proyecto</t>
+  </si>
+  <si>
+    <t>Portafolio manager</t>
+  </si>
+  <si>
+    <t>todas las  minutas de trabajo se encuentra programado como parte de la agenda el punto de acuerdos, para establecer fechas, responsables, actividades y seguimiento de las tareas pendientes.</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>programador</t>
+  </si>
+  <si>
+    <t>Se restructuró  el cronograma que las  actividades y tiempos, se reajusten y coincidan.</t>
+  </si>
+  <si>
+    <t>Los nuevos cambios a los requisitos se ajustan  a los anteriores.</t>
+  </si>
+  <si>
+    <t>nuevo analisis de los datos para  el rediseño de las intefaces ajustandola a los nuevos datos en la base de datos.</t>
+  </si>
+  <si>
+    <t>nueva estructura de los datos  ajustando la base de datos de forma que se ajustaron los nuevos datos al diseño existente</t>
+  </si>
+  <si>
+    <t>Rediseñar las interfaces con base  a los requerimientos de software Aplicación de la norma ISO 9126 en el criterio de Usabilidad.</t>
   </si>
   <si>
     <t>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
-•someter nuevamente a pruebas los módulos donde se reportaron fallas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acoplar los requerimientos nuevos o cambios  existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </t>
-  </si>
-  <si>
-    <t>Comunicación</t>
-  </si>
-  <si>
-    <t>todos los entregables del proyecto</t>
-  </si>
-  <si>
-    <t>Portafolio manager</t>
-  </si>
-  <si>
-    <t>todas las  minutas de trabajo se encuentra programado como parte de la agenda el punto de acuerdos, para establecer fechas, responsables, actividades y seguimiento de las tareas pendientes.</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>programador</t>
-  </si>
-  <si>
-    <t>Se restructuró  el cronograma que las  actividades y tiempos, se reajusten y coincidan.</t>
-  </si>
-  <si>
-    <t>Los nuevos cambios a los requisitos se ajustan  a los anteriores.</t>
-  </si>
-  <si>
-    <t>nuevo analisis de los datos para  el rediseño de las intefaces ajustandola a los nuevos datos en la base de datos.</t>
-  </si>
-  <si>
-    <t>nueva estructura de los datos  ajustando la base de datos de forma que se ajustaron los nuevos datos al diseño existente</t>
+•someter nuevamente a pruebas los módulos donde se reportaron fallas                           Seguimiento a la aplicación de la norma ISO 9126 en el criterio de eficiencia de desempeño</t>
   </si>
 </sst>
 </file>
@@ -1644,6 +1644,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1653,58 +1698,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2066,27 +2066,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="D21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
-    <col min="12" max="1023" width="8.5546875" customWidth="1"/>
+    <col min="12" max="1023" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="136" t="s">
         <v>79</v>
       </c>
@@ -2100,7 +2100,7 @@
       <c r="J1" s="137"/>
       <c r="K1" s="138"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2112,7 +2112,7 @@
       <c r="J2" s="27"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2124,7 +2124,7 @@
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="143" t="s">
         <v>0</v>
       </c>
@@ -2140,7 +2140,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="14"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>5</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="14"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -2188,7 +2188,7 @@
       <c r="J6" s="13"/>
       <c r="K6" s="14"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="J7" s="13"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>2</v>
       </c>
@@ -2236,7 +2236,7 @@
       <c r="J8" s="13"/>
       <c r="K8" s="14"/>
     </row>
-    <row r="9" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>1</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2272,7 +2272,7 @@
       <c r="J10" s="13"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -2284,7 +2284,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -2296,7 +2296,7 @@
       <c r="J12" s="13"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="141" t="s">
         <v>21</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="135"/>
       <c r="C14" s="135"/>
       <c r="D14" s="135"/>
@@ -2328,7 +2328,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>24</v>
       </c>
@@ -2360,12 +2360,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="97">
         <v>1</v>
       </c>
       <c r="C16" s="98" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D16" s="120" t="s">
         <v>103</v>
@@ -2393,7 +2393,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="20">
         <v>2</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="22">
         <v>3</v>
       </c>
@@ -2456,10 +2456,10 @@
         <v>12</v>
       </c>
       <c r="K18" s="118" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="70.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="22">
         <v>4</v>
       </c>
@@ -2489,10 +2489,10 @@
         <v>6</v>
       </c>
       <c r="K19" s="119" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="22">
         <v>5</v>
       </c>
@@ -2500,16 +2500,16 @@
         <v>92</v>
       </c>
       <c r="D20" s="128" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="129" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="129" t="s">
+      <c r="F20" s="130" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="131" t="s">
         <v>117</v>
-      </c>
-      <c r="F20" s="130" t="s">
-        <v>119</v>
-      </c>
-      <c r="G20" s="131" t="s">
-        <v>118</v>
       </c>
       <c r="H20" s="112">
         <v>3</v>
@@ -2522,10 +2522,10 @@
         <v>12</v>
       </c>
       <c r="K20" s="119" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="175.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="22">
         <v>6</v>
       </c>
@@ -2555,10 +2555,10 @@
         <v>15</v>
       </c>
       <c r="K21" s="118" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="22">
         <v>7</v>
       </c>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="K22" s="99"/>
     </row>
-    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="22">
         <v>8</v>
       </c>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="K23" s="99"/>
     </row>
-    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="22">
         <v>9</v>
       </c>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="K24" s="99"/>
     </row>
-    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="22">
         <v>10</v>
       </c>
@@ -2642,7 +2642,7 @@
       </c>
       <c r="K25" s="99"/>
     </row>
-    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="22">
         <v>11</v>
       </c>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="K26" s="99"/>
     </row>
-    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="22">
         <v>12</v>
       </c>
@@ -2684,7 +2684,7 @@
       </c>
       <c r="K27" s="99"/>
     </row>
-    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="22">
         <v>13</v>
       </c>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="K28" s="99"/>
     </row>
-    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="22">
         <v>14</v>
       </c>
@@ -2726,7 +2726,7 @@
       </c>
       <c r="K29" s="99"/>
     </row>
-    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="24">
         <v>15</v>
       </c>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="K30" s="100"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -2759,7 +2759,7 @@
       <c r="J31" s="13"/>
       <c r="K31" s="14"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2771,7 +2771,7 @@
       <c r="J32" s="13"/>
       <c r="K32" s="14"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2783,7 +2783,7 @@
       <c r="J33" s="13"/>
       <c r="K33" s="14"/>
     </row>
-    <row r="34" spans="2:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="74"/>
       <c r="C34" s="75"/>
       <c r="D34" s="75"/>
@@ -2826,20 +2826,20 @@
       <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2853,23 +2853,23 @@
       <c r="L2" s="27"/>
       <c r="M2" s="28"/>
     </row>
-    <row r="3" spans="2:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="12"/>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
+      <c r="L3" s="159"/>
       <c r="M3" s="14"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -2883,7 +2883,7 @@
       <c r="L4" s="13"/>
       <c r="M4" s="14"/>
     </row>
-    <row r="5" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="29" t="s">
         <v>0</v>
@@ -2902,16 +2902,16 @@
       <c r="I5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="145" t="s">
+      <c r="J5" s="160" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="145"/>
+      <c r="K5" s="160"/>
       <c r="L5" s="34" t="s">
         <v>36</v>
       </c>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="2:17" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
       <c r="C6" s="35" t="s">
         <v>37</v>
@@ -2930,17 +2930,17 @@
       <c r="I6" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="146" t="s">
+      <c r="J6" s="161" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="146"/>
+      <c r="K6" s="161"/>
       <c r="L6" s="37">
         <f>16/25*100</f>
         <v>64</v>
       </c>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="C7" s="40" t="s">
         <v>41</v>
@@ -2959,17 +2959,17 @@
       <c r="I7" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="147" t="s">
+      <c r="J7" s="155" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="147"/>
+      <c r="K7" s="155"/>
       <c r="L7" s="42">
         <f>15/25*100</f>
         <v>60</v>
       </c>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
       <c r="C8" s="40" t="s">
         <v>45</v>
@@ -2988,17 +2988,17 @@
       <c r="I8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="147" t="s">
+      <c r="J8" s="155" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="147"/>
+      <c r="K8" s="155"/>
       <c r="L8" s="42">
         <f>12/25*100</f>
         <v>48</v>
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
       <c r="C9" s="40" t="s">
         <v>47</v>
@@ -3017,17 +3017,17 @@
       <c r="I9" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="147" t="s">
+      <c r="J9" s="155" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="147"/>
+      <c r="K9" s="155"/>
       <c r="L9" s="42">
         <f>8/25*100</f>
         <v>32</v>
       </c>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="45" t="s">
         <v>49</v>
@@ -3046,10 +3046,10 @@
       <c r="I10" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="148" t="s">
+      <c r="J10" s="156" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="148"/>
+      <c r="K10" s="156"/>
       <c r="L10" s="47">
         <f>5/25*100</f>
         <v>20</v>
@@ -3060,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="49"/>
       <c r="D11" s="13"/>
@@ -3074,7 +3074,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -3088,17 +3088,17 @@
       <c r="L12" s="13"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="2:17" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="149" t="s">
+      <c r="D13" s="157" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="149"/>
+      <c r="E13" s="157"/>
       <c r="F13" s="51" t="s">
         <v>54</v>
       </c>
@@ -3122,23 +3122,23 @@
       </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="2:17" ht="88.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" ht="88.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12"/>
       <c r="C14" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B16)</f>
         <v>R1</v>
       </c>
-      <c r="D14" s="150" t="str">
+      <c r="D14" s="158" t="str">
         <f>Matriz!E16</f>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="E14" s="150"/>
+      <c r="E14" s="158"/>
       <c r="F14" s="54" t="str">
         <f>Matriz!F16</f>
         <v xml:space="preserve">Mala comunicación, descuerdos en el equipo y trabajo disperso. </v>
       </c>
       <c r="G14" s="132" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H14" s="54">
         <f>Matriz!H16</f>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="2:17" ht="79.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12"/>
       <c r="C15" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B17)</f>
@@ -3202,7 +3202,7 @@
       </c>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12"/>
       <c r="C16" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B18)</f>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:13" ht="86.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12"/>
       <c r="C17" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B19)</f>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="2:13" ht="95.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="95.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12"/>
       <c r="C18" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B20)</f>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:13" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="12"/>
       <c r="C19" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B21)</f>
@@ -3362,7 +3362,7 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="12"/>
       <c r="C20" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B22)</f>
@@ -3400,7 +3400,7 @@
       </c>
       <c r="M20" s="14"/>
     </row>
-    <row r="21" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="12"/>
       <c r="C21" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B23)</f>
@@ -3438,7 +3438,7 @@
       </c>
       <c r="M21" s="14"/>
     </row>
-    <row r="22" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
       <c r="C22" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B24)</f>
@@ -3476,7 +3476,7 @@
       </c>
       <c r="M22" s="14"/>
     </row>
-    <row r="23" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
       <c r="C23" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B25)</f>
@@ -3514,7 +3514,7 @@
       </c>
       <c r="M23" s="14"/>
     </row>
-    <row r="24" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
       <c r="C24" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B26)</f>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="M24" s="14"/>
     </row>
-    <row r="25" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="12"/>
       <c r="C25" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B27)</f>
@@ -3590,7 +3590,7 @@
       </c>
       <c r="M25" s="14"/>
     </row>
-    <row r="26" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
       <c r="C26" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B28)</f>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="M26" s="14"/>
     </row>
-    <row r="27" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
       <c r="C27" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B29)</f>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="M27" s="14"/>
     </row>
-    <row r="28" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
       <c r="C28" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B30)</f>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="M28" s="14"/>
     </row>
-    <row r="29" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3718,7 +3718,7 @@
       <c r="L29" s="13"/>
       <c r="M29" s="14"/>
     </row>
-    <row r="30" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="152" t="s">
         <v>61</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="L30" s="152"/>
       <c r="M30" s="152"/>
     </row>
-    <row r="31" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -3748,7 +3748,7 @@
       <c r="L31" s="13"/>
       <c r="M31" s="14"/>
     </row>
-    <row r="32" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="12"/>
       <c r="C32" s="61" t="s">
         <v>52</v>
@@ -3778,17 +3778,17 @@
       <c r="L32" s="154"/>
       <c r="M32" s="14"/>
     </row>
-    <row r="33" spans="2:13" ht="163.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" ht="163.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="12"/>
       <c r="C33" s="63" t="str">
         <f t="shared" ref="C33:D47" si="3">C14</f>
         <v>R1</v>
       </c>
-      <c r="D33" s="155" t="str">
+      <c r="D33" s="148" t="str">
         <f t="shared" si="3"/>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="E33" s="155"/>
+      <c r="E33" s="148"/>
       <c r="F33" s="65" t="str">
         <f t="shared" ref="F33:F47" si="4">K14</f>
         <v>ALTO</v>
@@ -3805,27 +3805,27 @@
         <v>67</v>
       </c>
       <c r="J33" s="64" t="s">
-        <v>125</v>
-      </c>
-      <c r="K33" s="156" t="str">
+        <v>123</v>
+      </c>
+      <c r="K33" s="149" t="str">
         <f>Matriz!K16</f>
         <v>•Realización de reuniones sobre avances del proyecto
 •Realizar acuerdos y trabajar en un punto medio de opiniones</v>
       </c>
-      <c r="L33" s="156"/>
+      <c r="L33" s="149"/>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="2:13" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
       <c r="C34" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R2</v>
       </c>
-      <c r="D34" s="157" t="str">
+      <c r="D34" s="150" t="str">
         <f t="shared" si="3"/>
         <v>Tiempos incongruentes y fechas mal planeadas ,Organización ineficiente</v>
       </c>
-      <c r="E34" s="157"/>
+      <c r="E34" s="150"/>
       <c r="F34" s="67" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
@@ -3841,26 +3841,26 @@
         <v>67</v>
       </c>
       <c r="J34" s="68" t="s">
-        <v>125</v>
-      </c>
-      <c r="K34" s="158" t="str">
+        <v>123</v>
+      </c>
+      <c r="K34" s="147" t="str">
         <f>Matriz!K17</f>
         <v>Revisar actividades con fechas y ajustarlos a tiempos del proyecto, utilizar un repositorio para el almacenamiento de la información.</v>
       </c>
-      <c r="L34" s="158"/>
+      <c r="L34" s="147"/>
       <c r="M34" s="14"/>
     </row>
-    <row r="35" spans="2:13" ht="125.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" ht="125.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
       <c r="C35" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R3</v>
       </c>
-      <c r="D35" s="159" t="str">
+      <c r="D35" s="146" t="str">
         <f t="shared" si="3"/>
         <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
       </c>
-      <c r="E35" s="159"/>
+      <c r="E35" s="146"/>
       <c r="F35" s="70" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
@@ -3876,26 +3876,26 @@
         <v>67</v>
       </c>
       <c r="J35" s="69" t="s">
-        <v>125</v>
-      </c>
-      <c r="K35" s="158" t="str">
+        <v>123</v>
+      </c>
+      <c r="K35" s="147" t="str">
         <f>Matriz!K18</f>
         <v xml:space="preserve">Acoplar los requerimientos nuevos o cambios  existentes de forma clara y  eficiente  para cumplir la funcionalidad planeada </v>
       </c>
-      <c r="L35" s="158"/>
+      <c r="L35" s="147"/>
       <c r="M35" s="14"/>
     </row>
-    <row r="36" spans="2:13" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="12"/>
       <c r="C36" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R4</v>
       </c>
-      <c r="D36" s="159" t="str">
+      <c r="D36" s="146" t="str">
         <f t="shared" si="3"/>
         <v>interpretación erronea de las ventanas e interfaces</v>
       </c>
-      <c r="E36" s="159"/>
+      <c r="E36" s="146"/>
       <c r="F36" s="67" t="str">
         <f t="shared" si="4"/>
         <v>BAJO</v>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="H36" s="88" t="str">
         <f>Matriz!K19</f>
-        <v>Rediseñar las interfaces con base  a los requerimientos de software</v>
+        <v>Rediseñar las interfaces con base  a los requerimientos de software Aplicación de la norma ISO 9126 en el criterio de Usabilidad.</v>
       </c>
       <c r="I36" s="64" t="s">
         <v>67</v>
@@ -3913,24 +3913,24 @@
       <c r="J36" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="K36" s="158" t="str">
+      <c r="K36" s="147" t="str">
         <f>Matriz!K19</f>
-        <v>Rediseñar las interfaces con base  a los requerimientos de software</v>
-      </c>
-      <c r="L36" s="158"/>
+        <v>Rediseñar las interfaces con base  a los requerimientos de software Aplicación de la norma ISO 9126 en el criterio de Usabilidad.</v>
+      </c>
+      <c r="L36" s="147"/>
       <c r="M36" s="14"/>
     </row>
-    <row r="37" spans="2:13" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
       <c r="C37" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R5</v>
       </c>
-      <c r="D37" s="159" t="str">
+      <c r="D37" s="146" t="str">
         <f t="shared" si="3"/>
         <v>Estructuración erronea de los datos, tablas mal relacionadas</v>
       </c>
-      <c r="E37" s="159"/>
+      <c r="E37" s="146"/>
       <c r="F37" s="70" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
@@ -3948,63 +3948,63 @@
       <c r="J37" s="69" t="s">
         <v>90</v>
       </c>
-      <c r="K37" s="158" t="str">
+      <c r="K37" s="147" t="str">
         <f>Matriz!K20</f>
         <v>Redefinir la arquitectura lógica llevando a cabo un analisis produndo para lograr  relaciones de tablas correctas con base a los procesos de la empresa</v>
       </c>
-      <c r="L37" s="158"/>
+      <c r="L37" s="147"/>
       <c r="M37" s="14"/>
     </row>
-    <row r="38" spans="2:13" ht="194.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" ht="194.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
       <c r="C38" s="71" t="str">
         <f t="shared" si="3"/>
         <v>R6</v>
       </c>
-      <c r="D38" s="160" t="str">
+      <c r="D38" s="144" t="str">
         <f t="shared" si="3"/>
         <v>Pruebas ineficientes</v>
       </c>
-      <c r="E38" s="160"/>
+      <c r="E38" s="144"/>
       <c r="F38" s="72" t="str">
         <f t="shared" si="4"/>
         <v>ALTO</v>
       </c>
       <c r="G38" s="73" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H38" s="88" t="str">
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
-•someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
+•someter nuevamente a pruebas los módulos donde se reportaron fallas                           Seguimiento a la aplicación de la norma ISO 9126 en el criterio de eficiencia de desempeño</v>
       </c>
       <c r="I38" s="64" t="s">
         <v>67</v>
       </c>
       <c r="J38" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="K38" s="161" t="str">
+        <v>126</v>
+      </c>
+      <c r="K38" s="145" t="str">
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
-•someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
-      </c>
-      <c r="L38" s="161"/>
+•someter nuevamente a pruebas los módulos donde se reportaron fallas                           Seguimiento a la aplicación de la norma ISO 9126 en el criterio de eficiencia de desempeño</v>
+      </c>
+      <c r="L38" s="145"/>
       <c r="M38" s="14"/>
     </row>
-    <row r="39" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="12"/>
       <c r="C39" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R7</v>
       </c>
-      <c r="D39" s="160">
+      <c r="D39" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E39" s="160"/>
+      <c r="E39" s="144"/>
       <c r="F39" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4018,24 +4018,24 @@
         <v>67</v>
       </c>
       <c r="J39" s="73"/>
-      <c r="K39" s="161">
+      <c r="K39" s="145">
         <f>Matriz!K22</f>
         <v>0</v>
       </c>
-      <c r="L39" s="161"/>
+      <c r="L39" s="145"/>
       <c r="M39" s="14"/>
     </row>
-    <row r="40" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="C40" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R8</v>
       </c>
-      <c r="D40" s="160">
+      <c r="D40" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E40" s="160"/>
+      <c r="E40" s="144"/>
       <c r="F40" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4049,24 +4049,24 @@
         <v>67</v>
       </c>
       <c r="J40" s="73"/>
-      <c r="K40" s="161">
+      <c r="K40" s="145">
         <f>Matriz!K23</f>
         <v>0</v>
       </c>
-      <c r="L40" s="161"/>
+      <c r="L40" s="145"/>
       <c r="M40" s="14"/>
     </row>
-    <row r="41" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
       <c r="C41" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R9</v>
       </c>
-      <c r="D41" s="160">
+      <c r="D41" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E41" s="160"/>
+      <c r="E41" s="144"/>
       <c r="F41" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4080,24 +4080,24 @@
         <v>67</v>
       </c>
       <c r="J41" s="73"/>
-      <c r="K41" s="161">
+      <c r="K41" s="145">
         <f>Matriz!K24</f>
         <v>0</v>
       </c>
-      <c r="L41" s="161"/>
+      <c r="L41" s="145"/>
       <c r="M41" s="14"/>
     </row>
-    <row r="42" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
       <c r="C42" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R10</v>
       </c>
-      <c r="D42" s="160">
+      <c r="D42" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E42" s="160"/>
+      <c r="E42" s="144"/>
       <c r="F42" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4111,24 +4111,24 @@
         <v>67</v>
       </c>
       <c r="J42" s="73"/>
-      <c r="K42" s="161">
+      <c r="K42" s="145">
         <f>Matriz!K25</f>
         <v>0</v>
       </c>
-      <c r="L42" s="161"/>
+      <c r="L42" s="145"/>
       <c r="M42" s="14"/>
     </row>
-    <row r="43" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
       <c r="C43" s="71" t="str">
         <f t="shared" si="3"/>
         <v>R11</v>
       </c>
-      <c r="D43" s="160">
+      <c r="D43" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E43" s="160"/>
+      <c r="E43" s="144"/>
       <c r="F43" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4142,24 +4142,24 @@
         <v>67</v>
       </c>
       <c r="J43" s="73"/>
-      <c r="K43" s="161">
+      <c r="K43" s="145">
         <f>Matriz!K26</f>
         <v>0</v>
       </c>
-      <c r="L43" s="161"/>
+      <c r="L43" s="145"/>
       <c r="M43" s="14"/>
     </row>
-    <row r="44" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="C44" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R12</v>
       </c>
-      <c r="D44" s="160">
+      <c r="D44" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E44" s="160"/>
+      <c r="E44" s="144"/>
       <c r="F44" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4173,24 +4173,24 @@
         <v>67</v>
       </c>
       <c r="J44" s="73"/>
-      <c r="K44" s="161">
+      <c r="K44" s="145">
         <f>Matriz!K27</f>
         <v>0</v>
       </c>
-      <c r="L44" s="161"/>
+      <c r="L44" s="145"/>
       <c r="M44" s="14"/>
     </row>
-    <row r="45" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
       <c r="C45" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R13</v>
       </c>
-      <c r="D45" s="160">
+      <c r="D45" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E45" s="160"/>
+      <c r="E45" s="144"/>
       <c r="F45" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4204,24 +4204,24 @@
         <v>67</v>
       </c>
       <c r="J45" s="73"/>
-      <c r="K45" s="161">
+      <c r="K45" s="145">
         <f>Matriz!K28</f>
         <v>0</v>
       </c>
-      <c r="L45" s="161"/>
+      <c r="L45" s="145"/>
       <c r="M45" s="14"/>
     </row>
-    <row r="46" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="C46" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R14</v>
       </c>
-      <c r="D46" s="160">
+      <c r="D46" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E46" s="160"/>
+      <c r="E46" s="144"/>
       <c r="F46" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4235,24 +4235,24 @@
         <v>67</v>
       </c>
       <c r="J46" s="73"/>
-      <c r="K46" s="161">
+      <c r="K46" s="145">
         <f>Matriz!K29</f>
         <v>0</v>
       </c>
-      <c r="L46" s="161"/>
+      <c r="L46" s="145"/>
       <c r="M46" s="14"/>
     </row>
-    <row r="47" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="C47" s="66" t="str">
         <f t="shared" si="3"/>
         <v>R15</v>
       </c>
-      <c r="D47" s="160">
+      <c r="D47" s="144">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E47" s="160"/>
+      <c r="E47" s="144"/>
       <c r="F47" s="72" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4266,14 +4266,14 @@
         <v>67</v>
       </c>
       <c r="J47" s="73"/>
-      <c r="K47" s="161">
+      <c r="K47" s="145">
         <f>Matriz!K30</f>
         <v>0</v>
       </c>
-      <c r="L47" s="161"/>
+      <c r="L47" s="145"/>
       <c r="M47" s="14"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B48" s="12"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
@@ -4287,7 +4287,7 @@
       <c r="L48" s="13"/>
       <c r="M48" s="14"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B49" s="12"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
@@ -4301,7 +4301,7 @@
       <c r="L49" s="13"/>
       <c r="M49" s="14"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B50" s="74"/>
       <c r="C50" s="75"/>
       <c r="D50" s="75"/>
@@ -4317,62 +4317,62 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="K44:L44"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K45:L45"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="K47:L47"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B30:M30"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="L14:L28">
     <cfRule type="colorScale" priority="2">
@@ -4430,35 +4430,35 @@
       <selection activeCell="M13" sqref="M13:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="11.5546875"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="1" max="7" width="11.5703125"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="11" width="11.5546875"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="1025" width="11.5546875"/>
+    <col min="10" max="11" width="11.5703125"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="162" t="s">
+    <row r="4" spans="3:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="162"/>
-      <c r="E5" s="162"/>
-      <c r="F5" s="162"/>
-      <c r="G5" s="162"/>
-      <c r="H5" s="162"/>
-      <c r="I5" s="162"/>
-      <c r="J5" s="162"/>
-      <c r="K5" s="162"/>
-      <c r="L5" s="162"/>
-      <c r="M5" s="162"/>
-      <c r="N5" s="162"/>
-      <c r="O5" s="162"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="163"/>
+      <c r="O5" s="163"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -4473,15 +4473,15 @@
       <c r="N6" s="13"/>
       <c r="O6" s="14"/>
     </row>
-    <row r="7" spans="3:15" ht="33.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:15" ht="33.200000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="12"/>
       <c r="D7" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="163" t="s">
+      <c r="E7" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="163"/>
+      <c r="F7" s="164"/>
       <c r="G7" s="77" t="s">
         <v>62</v>
       </c>
@@ -4500,23 +4500,23 @@
       <c r="L7" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="163" t="s">
+      <c r="M7" s="164" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="163"/>
+      <c r="N7" s="164"/>
       <c r="O7" s="14"/>
     </row>
-    <row r="8" spans="3:15" ht="146.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" ht="146.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="12"/>
       <c r="D8" s="78" t="str">
         <f>'Cualitativo '!C33</f>
         <v>R1</v>
       </c>
-      <c r="E8" s="164" t="str">
+      <c r="E8" s="162" t="str">
         <f>'Cualitativo '!D33</f>
         <v>no trabajar eficientemente</v>
       </c>
-      <c r="F8" s="164"/>
+      <c r="F8" s="162"/>
       <c r="G8" s="80" t="str">
         <f>'Cualitativo '!F33</f>
         <v>ALTO</v>
@@ -4540,23 +4540,23 @@
         <f>'Cualitativo '!J33</f>
         <v>Portafolio manager</v>
       </c>
-      <c r="M8" s="164" t="s">
-        <v>126</v>
-      </c>
-      <c r="N8" s="164"/>
+      <c r="M8" s="162" t="s">
+        <v>124</v>
+      </c>
+      <c r="N8" s="162"/>
       <c r="O8" s="14"/>
     </row>
-    <row r="9" spans="3:15" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" ht="113.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="12"/>
       <c r="D9" s="78" t="str">
         <f>'Cualitativo '!C34</f>
         <v>R2</v>
       </c>
-      <c r="E9" s="164" t="str">
+      <c r="E9" s="162" t="str">
         <f>'Cualitativo '!D34</f>
         <v>Tiempos incongruentes y fechas mal planeadas ,Organización ineficiente</v>
       </c>
-      <c r="F9" s="164"/>
+      <c r="F9" s="162"/>
       <c r="G9" s="80" t="str">
         <f>'Cualitativo '!F34</f>
         <v>MODERADO</v>
@@ -4579,23 +4579,23 @@
         <f>'Cualitativo '!J34</f>
         <v>Portafolio manager</v>
       </c>
-      <c r="M9" s="164" t="s">
-        <v>129</v>
-      </c>
-      <c r="N9" s="164"/>
+      <c r="M9" s="162" t="s">
+        <v>127</v>
+      </c>
+      <c r="N9" s="162"/>
       <c r="O9" s="14"/>
     </row>
-    <row r="10" spans="3:15" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" ht="114.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="12"/>
       <c r="D10" s="78" t="str">
         <f>'Cualitativo '!C35</f>
         <v>R3</v>
       </c>
-      <c r="E10" s="164" t="str">
+      <c r="E10" s="162" t="str">
         <f>'Cualitativo '!D35</f>
         <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
       </c>
-      <c r="F10" s="164"/>
+      <c r="F10" s="162"/>
       <c r="G10" s="80" t="str">
         <f>'Cualitativo '!F35</f>
         <v>MODERADO</v>
@@ -4618,23 +4618,23 @@
         <f>'Cualitativo '!J35</f>
         <v>Portafolio manager</v>
       </c>
-      <c r="M10" s="164" t="s">
-        <v>130</v>
-      </c>
-      <c r="N10" s="164"/>
+      <c r="M10" s="162" t="s">
+        <v>128</v>
+      </c>
+      <c r="N10" s="162"/>
       <c r="O10" s="14"/>
     </row>
-    <row r="11" spans="3:15" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" ht="92.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="12"/>
       <c r="D11" s="78" t="str">
         <f>'Cualitativo '!C36</f>
         <v>R4</v>
       </c>
-      <c r="E11" s="164" t="str">
+      <c r="E11" s="162" t="str">
         <f>'Cualitativo '!D36</f>
         <v>interpretación erronea de las ventanas e interfaces</v>
       </c>
-      <c r="F11" s="164"/>
+      <c r="F11" s="162"/>
       <c r="G11" s="80" t="str">
         <f>'Cualitativo '!F36</f>
         <v>BAJO</v>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="I11" s="79" t="str">
         <f>Matriz!K19</f>
-        <v>Rediseñar las interfaces con base  a los requerimientos de software</v>
+        <v>Rediseñar las interfaces con base  a los requerimientos de software Aplicación de la norma ISO 9126 en el criterio de Usabilidad.</v>
       </c>
       <c r="J11" s="134" t="s">
         <v>74</v>
@@ -4656,23 +4656,23 @@
       <c r="L11" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="164" t="s">
-        <v>131</v>
-      </c>
-      <c r="N11" s="164"/>
+      <c r="M11" s="162" t="s">
+        <v>129</v>
+      </c>
+      <c r="N11" s="162"/>
       <c r="O11" s="14"/>
     </row>
-    <row r="12" spans="3:15" ht="137.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" ht="137.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="12"/>
       <c r="D12" s="78" t="str">
         <f>'Cualitativo '!C37</f>
         <v>R5</v>
       </c>
-      <c r="E12" s="164" t="str">
+      <c r="E12" s="162" t="str">
         <f>'Cualitativo '!D37</f>
         <v>Estructuración erronea de los datos, tablas mal relacionadas</v>
       </c>
-      <c r="F12" s="164"/>
+      <c r="F12" s="162"/>
       <c r="G12" s="80" t="str">
         <f>'Cualitativo '!F37</f>
         <v>MODERADO</v>
@@ -4695,23 +4695,23 @@
         <f>'Cualitativo '!J37</f>
         <v>Analista</v>
       </c>
-      <c r="M12" s="164" t="s">
-        <v>132</v>
-      </c>
-      <c r="N12" s="164"/>
+      <c r="M12" s="162" t="s">
+        <v>130</v>
+      </c>
+      <c r="N12" s="162"/>
       <c r="O12" s="14"/>
     </row>
-    <row r="13" spans="3:15" ht="212.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" ht="212.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="12"/>
       <c r="D13" s="78" t="str">
         <f>'Cualitativo '!C38</f>
         <v>R6</v>
       </c>
-      <c r="E13" s="164" t="str">
+      <c r="E13" s="162" t="str">
         <f>'Cualitativo '!D38</f>
         <v>Pruebas ineficientes</v>
       </c>
-      <c r="F13" s="164"/>
+      <c r="F13" s="162"/>
       <c r="G13" s="80" t="str">
         <f>'Cualitativo '!F38</f>
         <v>ALTO</v>
@@ -4724,7 +4724,7 @@
         <f>Matriz!K21</f>
         <v>•Realizar pruebas completas sobre cada módulo de la aplicación asegurandose de cumplir la funcionalidad principal
 •Darle seguimiento a cada falla encontrado
-•someter nuevamente a pruebas los módulos donde se reportaron fallas</v>
+•someter nuevamente a pruebas los módulos donde se reportaron fallas                           Seguimiento a la aplicación de la norma ISO 9126 en el criterio de eficiencia de desempeño</v>
       </c>
       <c r="J13" s="134"/>
       <c r="K13" s="79"/>
@@ -4732,21 +4732,21 @@
         <f>'Cualitativo '!J38</f>
         <v>programador</v>
       </c>
-      <c r="M13" s="164"/>
-      <c r="N13" s="164"/>
+      <c r="M13" s="162"/>
+      <c r="N13" s="162"/>
       <c r="O13" s="14"/>
     </row>
-    <row r="14" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="12"/>
       <c r="D14" s="78" t="str">
         <f>'Cualitativo '!C39</f>
         <v>R7</v>
       </c>
-      <c r="E14" s="164">
+      <c r="E14" s="162">
         <f>'Cualitativo '!D39</f>
         <v>0</v>
       </c>
-      <c r="F14" s="164"/>
+      <c r="F14" s="162"/>
       <c r="G14" s="80" t="str">
         <f>'Cualitativo '!F39</f>
         <v>MUY BAJO</v>
@@ -4765,21 +4765,21 @@
         <f>'Cualitativo '!J39</f>
         <v>0</v>
       </c>
-      <c r="M14" s="164"/>
-      <c r="N14" s="164"/>
+      <c r="M14" s="162"/>
+      <c r="N14" s="162"/>
       <c r="O14" s="14"/>
     </row>
-    <row r="15" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="12"/>
       <c r="D15" s="78" t="str">
         <f>'Cualitativo '!C40</f>
         <v>R8</v>
       </c>
-      <c r="E15" s="164">
+      <c r="E15" s="162">
         <f>'Cualitativo '!D40</f>
         <v>0</v>
       </c>
-      <c r="F15" s="164"/>
+      <c r="F15" s="162"/>
       <c r="G15" s="80" t="str">
         <f>'Cualitativo '!F40</f>
         <v>MUY BAJO</v>
@@ -4798,21 +4798,21 @@
         <f>'Cualitativo '!J40</f>
         <v>0</v>
       </c>
-      <c r="M15" s="164"/>
-      <c r="N15" s="164"/>
+      <c r="M15" s="162"/>
+      <c r="N15" s="162"/>
       <c r="O15" s="14"/>
     </row>
-    <row r="16" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="12"/>
       <c r="D16" s="78" t="str">
         <f>'Cualitativo '!C41</f>
         <v>R9</v>
       </c>
-      <c r="E16" s="164">
+      <c r="E16" s="162">
         <f>'Cualitativo '!D41</f>
         <v>0</v>
       </c>
-      <c r="F16" s="164"/>
+      <c r="F16" s="162"/>
       <c r="G16" s="80" t="str">
         <f>'Cualitativo '!F41</f>
         <v>MUY BAJO</v>
@@ -4831,21 +4831,21 @@
         <f>'Cualitativo '!J41</f>
         <v>0</v>
       </c>
-      <c r="M16" s="164"/>
-      <c r="N16" s="164"/>
+      <c r="M16" s="162"/>
+      <c r="N16" s="162"/>
       <c r="O16" s="14"/>
     </row>
-    <row r="17" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="12"/>
       <c r="D17" s="78" t="str">
         <f>'Cualitativo '!C42</f>
         <v>R10</v>
       </c>
-      <c r="E17" s="164">
+      <c r="E17" s="162">
         <f>'Cualitativo '!D42</f>
         <v>0</v>
       </c>
-      <c r="F17" s="164"/>
+      <c r="F17" s="162"/>
       <c r="G17" s="80" t="str">
         <f>'Cualitativo '!F42</f>
         <v>MUY BAJO</v>
@@ -4864,21 +4864,21 @@
         <f>'Cualitativo '!J42</f>
         <v>0</v>
       </c>
-      <c r="M17" s="164"/>
-      <c r="N17" s="164"/>
+      <c r="M17" s="162"/>
+      <c r="N17" s="162"/>
       <c r="O17" s="14"/>
     </row>
-    <row r="18" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="12"/>
       <c r="D18" s="78" t="str">
         <f>'Cualitativo '!C43</f>
         <v>R11</v>
       </c>
-      <c r="E18" s="164">
+      <c r="E18" s="162">
         <f>'Cualitativo '!D43</f>
         <v>0</v>
       </c>
-      <c r="F18" s="164"/>
+      <c r="F18" s="162"/>
       <c r="G18" s="80" t="str">
         <f>'Cualitativo '!F43</f>
         <v>MUY BAJO</v>
@@ -4897,21 +4897,21 @@
         <f>'Cualitativo '!J43</f>
         <v>0</v>
       </c>
-      <c r="M18" s="164"/>
-      <c r="N18" s="164"/>
+      <c r="M18" s="162"/>
+      <c r="N18" s="162"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="12"/>
       <c r="D19" s="78" t="str">
         <f>'Cualitativo '!C44</f>
         <v>R12</v>
       </c>
-      <c r="E19" s="164">
+      <c r="E19" s="162">
         <f>'Cualitativo '!D44</f>
         <v>0</v>
       </c>
-      <c r="F19" s="164"/>
+      <c r="F19" s="162"/>
       <c r="G19" s="80" t="str">
         <f>'Cualitativo '!F44</f>
         <v>MUY BAJO</v>
@@ -4930,21 +4930,21 @@
         <f>'Cualitativo '!J44</f>
         <v>0</v>
       </c>
-      <c r="M19" s="164"/>
-      <c r="N19" s="164"/>
+      <c r="M19" s="162"/>
+      <c r="N19" s="162"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="12"/>
       <c r="D20" s="78" t="str">
         <f>'Cualitativo '!C45</f>
         <v>R13</v>
       </c>
-      <c r="E20" s="164">
+      <c r="E20" s="162">
         <f>'Cualitativo '!D45</f>
         <v>0</v>
       </c>
-      <c r="F20" s="164"/>
+      <c r="F20" s="162"/>
       <c r="G20" s="80" t="str">
         <f>'Cualitativo '!F45</f>
         <v>MUY BAJO</v>
@@ -4963,21 +4963,21 @@
         <f>'Cualitativo '!J45</f>
         <v>0</v>
       </c>
-      <c r="M20" s="164"/>
-      <c r="N20" s="164"/>
+      <c r="M20" s="162"/>
+      <c r="N20" s="162"/>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="12"/>
       <c r="D21" s="78" t="str">
         <f>'Cualitativo '!C46</f>
         <v>R14</v>
       </c>
-      <c r="E21" s="164">
+      <c r="E21" s="162">
         <f>'Cualitativo '!D46</f>
         <v>0</v>
       </c>
-      <c r="F21" s="164"/>
+      <c r="F21" s="162"/>
       <c r="G21" s="80" t="str">
         <f>'Cualitativo '!F46</f>
         <v>MUY BAJO</v>
@@ -4996,21 +4996,21 @@
         <f>'Cualitativo '!J46</f>
         <v>0</v>
       </c>
-      <c r="M21" s="164"/>
-      <c r="N21" s="164"/>
+      <c r="M21" s="162"/>
+      <c r="N21" s="162"/>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="12"/>
       <c r="D22" s="78" t="str">
         <f>'Cualitativo '!C47</f>
         <v>R15</v>
       </c>
-      <c r="E22" s="164">
+      <c r="E22" s="162">
         <f>'Cualitativo '!D47</f>
         <v>0</v>
       </c>
-      <c r="F22" s="164"/>
+      <c r="F22" s="162"/>
       <c r="G22" s="80" t="str">
         <f>'Cualitativo '!F47</f>
         <v>MUY BAJO</v>
@@ -5029,11 +5029,11 @@
         <f>'Cualitativo '!J47</f>
         <v>0</v>
       </c>
-      <c r="M22" s="164"/>
-      <c r="N22" s="164"/>
+      <c r="M22" s="162"/>
+      <c r="N22" s="162"/>
       <c r="O22" s="14"/>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -5048,7 +5048,7 @@
       <c r="N23" s="13"/>
       <c r="O23" s="14"/>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -5063,7 +5063,7 @@
       <c r="N24" s="13"/>
       <c r="O24" s="14"/>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C25" s="74"/>
       <c r="D25" s="75"/>
       <c r="E25" s="75"/>
@@ -5080,6 +5080,29 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C5:O5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="M17:N17"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="E22:F22"/>
@@ -5090,29 +5113,6 @@
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C5:O5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="M8:N8"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5143,17 +5143,17 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="3.33203125" customWidth="1"/>
-    <col min="3" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" customWidth="1"/>
-    <col min="11" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" customWidth="1"/>
+    <col min="3" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+    <col min="11" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="165" t="s">
         <v>0</v>
       </c>
@@ -5186,7 +5186,7 @@
       <c r="M5" s="83"/>
       <c r="N5" s="83"/>
     </row>
-    <row r="6" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="165"/>
       <c r="C6" s="82">
         <v>4</v>
@@ -5217,7 +5217,7 @@
       <c r="M6" s="83"/>
       <c r="N6" s="83"/>
     </row>
-    <row r="7" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="165"/>
       <c r="C7" s="82">
         <v>3</v>
@@ -5248,7 +5248,7 @@
       <c r="M7" s="83"/>
       <c r="N7" s="83"/>
     </row>
-    <row r="8" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="165"/>
       <c r="C8" s="82">
         <v>2</v>
@@ -5279,7 +5279,7 @@
       <c r="M8" s="83"/>
       <c r="N8" s="83"/>
     </row>
-    <row r="9" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="165"/>
       <c r="C9" s="82">
         <v>1</v>
@@ -5310,7 +5310,7 @@
       <c r="M9" s="83"/>
       <c r="N9" s="83"/>
     </row>
-    <row r="10" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="84"/>
       <c r="D10" s="85">
         <v>1</v>
@@ -5328,7 +5328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D11" s="166" t="s">
         <v>1</v>
       </c>
@@ -5359,12 +5359,12 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1025" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D6" s="167" t="s">
         <v>59</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D7" s="86" t="s">
         <v>67</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D8" s="87" t="s">
         <v>75</v>
       </c>
@@ -5391,13 +5391,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D9" s="87" t="s">
         <v>77</v>
       </c>
       <c r="E9" s="87"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D10" s="87" t="s">
         <v>78</v>
       </c>

</xml_diff>